<commit_message>
Correction on Login tests
</commit_message>
<xml_diff>
--- a/VectorMobileTests/src/test/resources/testDatas/fillForgotFormPasswordWithForbiddenCharacter.xlsx
+++ b/VectorMobileTests/src/test/resources/testDatas/fillForgotFormPasswordWithForbiddenCharacter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeang\workspace\riotmobiletests\src\test\java\testDatas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeang\workspace\vector-automated-tests.git\VectorMobileTests\src\test\resources\testDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,9 +47,6 @@
     <t>@</t>
   </si>
   <si>
-    <t>"&amp;)ç_'</t>
-  </si>
-  <si>
     <t>riotuser4@gmail.com</t>
   </si>
   <si>
@@ -59,10 +56,13 @@
     <t>4qdsf32q54sd32f1q3s5d4f3245qsf354q3s5d4f3q5s4df34q5sd3f4q3s5d4f3q54sdf354qsd3f4</t>
   </si>
   <si>
-    <t>%£$</t>
-  </si>
-  <si>
     <t>lopopqs44</t>
+  </si>
+  <si>
+    <t>/"&amp;)ç_'</t>
+  </si>
+  <si>
+    <t>([ç^</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +423,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -439,18 +439,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -461,24 +461,24 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>